<commit_message>
change the position whereby the test's row number is appended to the received and approved file name.
</commit_message>
<xml_diff>
--- a/ApprovalTests.MSTest/SampleData/data.xlsx
+++ b/ApprovalTests.MSTest/SampleData/data.xlsx
@@ -16,19 +16,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Values</t>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>octo</t>
   </si>
   <si>
     <t>cat</t>
   </si>
   <si>
-    <t>octo</t>
-  </si>
-  <si>
     <t>ftw</t>
-  </si>
-  <si>
-    <t>Row</t>
   </si>
 </sst>
 </file>
@@ -87,10 +87,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B4" totalsRowShown="0">
   <autoFilter ref="A1:B4"/>
   <tableColumns count="2">
-    <tableColumn id="2" name="Row"/>
-    <tableColumn id="1" name="Values"/>
+    <tableColumn id="1" name="Row"/>
+    <tableColumn id="2" name="Value"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -384,17 +384,17 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -410,7 +410,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -418,7 +418,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>